<commit_message>
Add new power config
</commit_message>
<xml_diff>
--- a/doc/重量估算.xlsx
+++ b/doc/重量估算.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="4s 2214配置" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="78">
   <si>
     <t>数量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1255,7 +1255,7 @@
                   <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220</c:v>
+                  <c:v>290</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1070</c:v>
@@ -1574,7 +1574,7 @@
                   <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1619</c:v>
+                  <c:v>1745</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>285</c:v>
@@ -5688,7 +5688,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5724,7 +5724,7 @@
         <xdr:cNvPr id="4" name="图表 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5765,7 +5765,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5803,7 +5803,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5846,7 +5846,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5884,7 +5884,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6788,8 +6788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6967,27 +6967,24 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>7</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="F7">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="H7" t="s">
-        <v>45</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
@@ -7270,11 +7267,11 @@
       </c>
       <c r="E18">
         <f>SUM(E2:E17)</f>
-        <v>2811</v>
+        <v>2881</v>
       </c>
       <c r="G18">
         <f>SUM(G2:G17)</f>
-        <v>6396</v>
+        <v>6522</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
@@ -7283,11 +7280,11 @@
       </c>
       <c r="E19">
         <f>E18*1.2</f>
-        <v>3373.2</v>
+        <v>3457.2</v>
       </c>
       <c r="G19">
         <f>G18*1.2</f>
-        <v>7675.2</v>
+        <v>7826.4</v>
       </c>
       <c r="H19" t="s">
         <v>41</v>
@@ -7343,11 +7340,11 @@
       </c>
       <c r="E27">
         <f>E7+E10</f>
-        <v>220</v>
+        <v>290</v>
       </c>
       <c r="G27">
         <f>G7+G10</f>
-        <v>1619</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
@@ -7375,8 +7372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>